<commit_message>
changed api and db design
</commit_message>
<xml_diff>
--- a/design/DB.xlsx
+++ b/design/DB.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKSPACE\JavaScript\MERN\DeliveryApp\deliveryApp\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects workspace\Delivery_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12336"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="93">
   <si>
     <t>int8</t>
   </si>
@@ -298,6 +298,15 @@
   </si>
   <si>
     <t>goods weight</t>
+  </si>
+  <si>
+    <t>status "IDLE" or "Processing"</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>order price</t>
   </si>
 </sst>
 </file>
@@ -731,20 +740,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="52.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="52.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -758,7 +767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>40</v>
       </c>
@@ -772,7 +781,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="2" t="s">
         <v>33</v>
@@ -784,7 +793,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>30</v>
@@ -796,7 +805,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>51</v>
@@ -808,7 +817,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>53</v>
@@ -820,7 +829,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>27</v>
@@ -832,7 +841,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>39</v>
       </c>
@@ -846,7 +855,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="3" t="s">
         <v>20</v>
@@ -858,7 +867,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="10"/>
       <c r="B10" s="2" t="s">
         <v>38</v>
@@ -870,7 +879,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="2" t="s">
         <v>36</v>
@@ -882,7 +891,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>34</v>
       </c>
@@ -896,7 +905,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="2" t="s">
         <v>33</v>
@@ -908,7 +917,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="2" t="s">
         <v>30</v>
@@ -920,19 +929,19 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
         <v>51</v>
@@ -944,7 +953,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="2" t="s">
         <v>27</v>
@@ -956,7 +965,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>25</v>
       </c>
@@ -970,7 +979,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="3" t="s">
         <v>22</v>
@@ -982,7 +991,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="3" t="s">
         <v>21</v>
@@ -994,7 +1003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
@@ -1006,7 +1015,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
         <v>17</v>
@@ -1018,7 +1027,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="2" t="s">
         <v>15</v>
@@ -1030,7 +1039,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
         <v>13</v>
@@ -1042,7 +1051,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
       <c r="B25" s="2" t="s">
         <v>61</v>
@@ -1054,7 +1063,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="10"/>
       <c r="B26" s="2" t="s">
         <v>63</v>
@@ -1066,7 +1075,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="10"/>
       <c r="B27" s="2" t="s">
         <v>64</v>
@@ -1078,7 +1087,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="2" t="s">
         <v>67</v>
@@ -1090,7 +1099,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="2" t="s">
         <v>69</v>
@@ -1102,7 +1111,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
       <c r="B30" s="2" t="s">
         <v>70</v>
@@ -1114,7 +1123,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="2" t="s">
         <v>11</v>
@@ -1126,7 +1135,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="4" t="s">
         <v>10</v>
@@ -1138,7 +1147,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="4" t="s">
         <v>86</v>
@@ -1150,7 +1159,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="4" t="s">
         <v>88</v>
@@ -1162,7 +1171,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="4" t="s">
         <v>55</v>
@@ -1174,7 +1183,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="4" t="s">
         <v>57</v>
@@ -1186,7 +1195,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="4" t="s">
         <v>59</v>
@@ -1198,7 +1207,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="2" t="s">
         <v>8</v>
@@ -1210,7 +1219,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="2" t="s">
         <v>3</v>
@@ -1222,264 +1231,276 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="C41" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="10"/>
-      <c r="B41" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
       <c r="B42" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10"/>
       <c r="B43" s="2" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
       <c r="B44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="10"/>
+      <c r="B45" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="C46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="10"/>
-      <c r="B46" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="10"/>
       <c r="B47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="10"/>
+      <c r="B48" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="C48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="C49" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="10"/>
-      <c r="B49" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="10"/>
       <c r="B50" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="10"/>
       <c r="B51" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="10"/>
+      <c r="B53" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B54" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C53" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="6" t="s">
+      <c r="C54" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
-      <c r="B54" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="8"/>
       <c r="B55" s="6" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>0</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="8"/>
       <c r="B56" s="6" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="8"/>
       <c r="B57" s="6" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="8"/>
       <c r="B58" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="8"/>
+      <c r="B59" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D58" s="6" t="s">
+      <c r="C59" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="9"/>
-      <c r="B59" s="6" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="9"/>
+      <c r="B60" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C60" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D60" s="6" t="s">
         <v>85</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="A48:A52"/>
+    <mergeCell ref="A54:A60"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A49:A53"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="A12:A17"/>
-    <mergeCell ref="A18:A39"/>
-    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A18:A40"/>
+    <mergeCell ref="A41:A45"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B9" location="Sheet1!B2" display="clientID"/>

</xml_diff>